<commit_message>
sprint backolog and products manage
</commit_message>
<xml_diff>
--- a/Sprint backlogs.xlsx
+++ b/Sprint backlogs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\Documents\GitHub\SaveTheWorld\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SaveTheWorld\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FA55F9-0621-4B98-B3A4-6BD477807D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813B7545-141B-4A25-9753-A177CBE8DB33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{67BB49A0-8FD9-BB42-AE2B-A18D387602E7}"/>
   </bookViews>
@@ -88,7 +88,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -106,7 +106,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="bg-BG"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -366,7 +366,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>73</c:v>
@@ -610,7 +610,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="bg-BG"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1060,7 +1060,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="bg-BG"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1321,7 +1321,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>80</c:v>
@@ -3339,9 +3339,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3379,7 +3379,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3485,7 +3485,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3638,7 +3638,7 @@
   <dimension ref="C21:E31"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3659,7 +3659,7 @@
         <v>80</v>
       </c>
       <c r="E22">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
@@ -3779,7 +3779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DD432C-1F96-DA40-A9D7-2B1B4FB2DA86}">
   <dimension ref="C7:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3863,7 +3863,7 @@
   <dimension ref="C7:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3909,7 +3909,7 @@
         <v>90</v>
       </c>
       <c r="E13" s="1">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">

</xml_diff>